<commit_message>
chore: add new Excel files and implement Google Drive API functionality in api_fetch.py
</commit_message>
<xml_diff>
--- a/TASK_3/TAsk_3-Files.xlsx
+++ b/TASK_3/TAsk_3-Files.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/midhun/Developer/Git/Orion_Intern_Journey/TASK_3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A99178B7-E916-3A42-B89F-D68DCFB8EB22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FD73F8-A81A-0146-B081-B836AC7568EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="10062025" sheetId="1" r:id="rId1"/>
@@ -363,7 +363,7 @@
       <code>counts_df=counts_df.T</code>
     </pythonScript>
     <pythonScript>
-      <code>counts_df.plot(kind='line', marker='o', figsize=(10,6))
+      <code>counts_df.plot(kind='bar', stacked=True, figsize=(10,10))
 plt.title('Trend of Execution Status Counts Over Dates')
 plt.xlabel('Date')
 plt.ylabel('Count')
@@ -944,9 +944,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -997,8 +1004,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1008,6 +1023,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -1045,26 +1066,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="20% - Accent1" xfId="4" builtinId="30"/>
     <cellStyle name="40% - Accent3" xfId="2" builtinId="39"/>
+    <cellStyle name="Explanatory Text" xfId="3" builtinId="53"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1086,15 +1119,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>4233</xdr:colOff>
+      <xdr:colOff>4232</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>118791</xdr:rowOff>
+      <xdr:rowOff>19097</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>757767</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>80434</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>806993</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>124510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1122,8 +1155,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6642100" y="8974924"/>
-          <a:ext cx="6375400" cy="3703910"/>
+          <a:off x="6578350" y="9407136"/>
+          <a:ext cx="7202564" cy="4513060"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1487,8 +1520,8 @@
     <v>22</v>
   </a>
   <a r="2">
-    <v>990</v>
-    <v>590</v>
+    <v>989</v>
+    <v>989</v>
   </a>
 </arrayData>
 </file>
@@ -1968,7 +2001,7 @@
   <rv s="2">
     <v>&lt;class 'PIL.PngImagePlugin.PngImageFile'&gt;</v>
     <v>PngImageFile</v>
-    <v>&lt;PIL.PngImagePlugin.PngImageFile image mode=RGBA size=990x590 at 0x7F9B996B7590&gt;</v>
+    <v>&lt;PIL.PngImagePlugin.PngImageFile image mode=RGBA size=989x989 at 0x7F99DA0FB290&gt;</v>
     <v>56</v>
     <v>2</v>
   </rv>
@@ -9329,15 +9362,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282EAF0B-A46B-0443-A423-FB0FE8A81679}">
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:S101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E101"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="30.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9354,7 +9390,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -9371,7 +9407,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -9388,7 +9424,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -9405,7 +9441,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -9422,7 +9458,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -9439,7 +9475,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -9455,8 +9491,16 @@
       <c r="E7" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -9472,8 +9516,16 @@
       <c r="E8" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -9489,8 +9541,16 @@
       <c r="E9" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -9506,8 +9566,16 @@
       <c r="E10" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -9523,8 +9591,16 @@
       <c r="E11" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -9540,8 +9616,16 @@
       <c r="E12" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -9557,8 +9641,16 @@
       <c r="E13" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -9574,8 +9666,16 @@
       <c r="E14" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -9591,8 +9691,16 @@
       <c r="E15" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -9608,8 +9716,16 @@
       <c r="E16" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -9625,8 +9741,16 @@
       <c r="E17" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -9642,8 +9766,16 @@
       <c r="E18" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -9659,8 +9791,16 @@
       <c r="E19" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -9676,8 +9816,16 @@
       <c r="E20" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -9693,8 +9841,16 @@
       <c r="E21" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -9710,8 +9866,16 @@
       <c r="E22" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -9727,8 +9891,16 @@
       <c r="E23" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -9744,8 +9916,16 @@
       <c r="E24" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -9761,8 +9941,16 @@
       <c r="E25" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -9778,8 +9966,16 @@
       <c r="E26" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -9795,8 +9991,16 @@
       <c r="E27" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -9812,8 +10016,16 @@
       <c r="E28" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="10"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -9829,8 +10041,16 @@
       <c r="E29" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="10"/>
+      <c r="S29" s="10"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -9846,8 +10066,16 @@
       <c r="E30" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10"/>
+      <c r="R30" s="10"/>
+      <c r="S30" s="10"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -9863,8 +10091,16 @@
       <c r="E31" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
+      <c r="R31" s="10"/>
+      <c r="S31" s="10"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -9880,8 +10116,16 @@
       <c r="E32" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="10"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="10"/>
+      <c r="R32" s="10"/>
+      <c r="S32" s="10"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -9897,8 +10141,16 @@
       <c r="E33" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
+      <c r="O33" s="10"/>
+      <c r="P33" s="10"/>
+      <c r="Q33" s="10"/>
+      <c r="R33" s="10"/>
+      <c r="S33" s="10"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -9915,7 +10167,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -9932,7 +10184,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -9949,7 +10201,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -9966,7 +10218,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -9983,7 +10235,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -10000,7 +10252,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -10017,7 +10269,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -10034,7 +10286,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -10051,7 +10303,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>46</v>
       </c>
@@ -10068,7 +10320,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -10085,7 +10337,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>48</v>
       </c>
@@ -10102,7 +10354,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -10119,7 +10371,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -10136,7 +10388,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -11062,19 +11314,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1345756A-7B60-E14F-9547-EADEB936F73C}">
-  <dimension ref="A1:P101"/>
+  <dimension ref="A1:Q101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="J78" sqref="J78"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="T29" sqref="T29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" customWidth="1"/>
+    <col min="4" max="4" width="114" customWidth="1"/>
+    <col min="5" max="5" width="36.5" customWidth="1"/>
     <col min="9" max="9" width="15.5" customWidth="1"/>
     <col min="10" max="10" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11090,8 +11346,18 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+    </row>
+    <row r="2" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -11107,13 +11373,20 @@
       <c r="E2" t="s">
         <v>156</v>
       </c>
+      <c r="H2" s="8"/>
       <c r="I2" s="4" t="s">
         <v>159</v>
       </c>
       <c r="J2" s="4"/>
-      <c r="K2" s="3"/>
-    </row>
-    <row r="3" spans="1:14" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="8"/>
+    </row>
+    <row r="3" spans="1:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -11129,8 +11402,10 @@
       <c r="E3" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H3" s="8"/>
+      <c r="Q3" s="8"/>
+    </row>
+    <row r="4" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -11146,15 +11421,23 @@
       <c r="E4" t="s">
         <v>158</v>
       </c>
+      <c r="H4" s="8"/>
       <c r="I4" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="J4" t="e" cm="1" vm="1">
+      <c r="J4" s="7" t="e" cm="1" vm="1">
         <f t="array" ref="J4">_xlfn._xlws.PY(0,1,'10062025'!E1:E101)</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="8"/>
+    </row>
+    <row r="5" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -11170,15 +11453,23 @@
       <c r="E5" t="s">
         <v>156</v>
       </c>
+      <c r="H5" s="8"/>
       <c r="I5" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="J5" t="e" cm="1" vm="2">
+      <c r="J5" s="7" t="e" cm="1" vm="2">
         <f t="array" ref="J5">_xlfn._xlws.PY(1,1,'11062025'!E1:E101)</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="8"/>
+    </row>
+    <row r="6" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -11194,15 +11485,23 @@
       <c r="E6" t="s">
         <v>155</v>
       </c>
+      <c r="H6" s="8"/>
       <c r="I6" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="J6" t="e" cm="1" vm="3">
+      <c r="J6" s="7" t="e" cm="1" vm="3">
         <f t="array" ref="J6">_xlfn._xlws.PY(2,1,'12062025'!E1:E101)</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="8"/>
+    </row>
+    <row r="7" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -11218,15 +11517,23 @@
       <c r="E7" t="s">
         <v>158</v>
       </c>
+      <c r="H7" s="8"/>
       <c r="I7" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="J7" t="e" cm="1" vm="4">
+      <c r="J7" s="7" t="e" cm="1" vm="4">
         <f t="array" ref="J7">_xlfn._xlws.PY(3,1,'13062025'!E1:E101)</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="8"/>
+    </row>
+    <row r="8" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -11242,15 +11549,23 @@
       <c r="E8" t="s">
         <v>157</v>
       </c>
+      <c r="H8" s="8"/>
       <c r="I8" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="J8" t="e" cm="1" vm="5">
+      <c r="J8" s="7" t="e" cm="1" vm="5">
         <f t="array" ref="J8">_xlfn._xlws.PY(4,1,'14062025'!E1:E101)</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="8"/>
+    </row>
+    <row r="9" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -11266,15 +11581,23 @@
       <c r="E9" t="s">
         <v>157</v>
       </c>
+      <c r="H9" s="8"/>
       <c r="I9" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="J9" t="e" cm="1" vm="6">
+      <c r="J9" s="7" t="e" cm="1" vm="6">
         <f t="array" ref="J9">_xlfn._xlws.PY(5,1,E1:E101)</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="8"/>
+    </row>
+    <row r="10" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -11290,8 +11613,16 @@
       <c r="E10" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" ht="30" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H10" s="8"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="8"/>
+    </row>
+    <row r="11" spans="1:17" ht="30" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -11307,6 +11638,7 @@
       <c r="E11" t="s">
         <v>155</v>
       </c>
+      <c r="H11" s="8"/>
       <c r="I11" s="4" t="s">
         <v>160</v>
       </c>
@@ -11315,8 +11647,11 @@
       <c r="L11" s="5"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
-    </row>
-    <row r="12" spans="1:14" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="8"/>
+    </row>
+    <row r="12" spans="1:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -11332,8 +11667,10 @@
       <c r="E12" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H12" s="8"/>
+      <c r="Q12" s="8"/>
+    </row>
+    <row r="13" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -11349,15 +11686,17 @@
       <c r="E13" t="s">
         <v>155</v>
       </c>
+      <c r="H13" s="8"/>
       <c r="I13" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="J13" t="e" cm="1" vm="7">
+      <c r="J13" s="7" t="e" cm="1" vm="7">
         <f t="array" ref="J13">_xlfn._xlws.PY(6,1)</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q13" s="8"/>
+    </row>
+    <row r="14" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -11373,15 +11712,17 @@
       <c r="E14" t="s">
         <v>155</v>
       </c>
+      <c r="H14" s="8"/>
       <c r="I14" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="J14" t="e" cm="1" vm="8">
+      <c r="J14" s="7" t="e" cm="1" vm="8">
         <f t="array" ref="J14">_xlfn._xlws.PY(7,1)</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q14" s="8"/>
+    </row>
+    <row r="15" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -11397,15 +11738,17 @@
       <c r="E15" t="s">
         <v>155</v>
       </c>
+      <c r="H15" s="8"/>
       <c r="I15" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="J15" t="e" cm="1" vm="9">
+      <c r="J15" s="7" t="e" cm="1" vm="9">
         <f t="array" ref="J15">_xlfn._xlws.PY(8,1)</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="Q15" s="8"/>
+    </row>
+    <row r="16" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -11421,15 +11764,17 @@
       <c r="E16" t="s">
         <v>158</v>
       </c>
+      <c r="H16" s="8"/>
       <c r="I16" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="J16" t="e" cm="1" vm="10">
+      <c r="J16" s="7" t="e" cm="1" vm="10">
         <f t="array" ref="J16">_xlfn._xlws.PY(9,1)</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q16" s="8"/>
+    </row>
+    <row r="17" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -11445,15 +11790,17 @@
       <c r="E17" t="s">
         <v>157</v>
       </c>
+      <c r="H17" s="8"/>
       <c r="I17" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="J17" t="e" cm="1" vm="11">
+      <c r="J17" s="7" t="e" cm="1" vm="11">
         <f t="array" ref="J17">_xlfn._xlws.PY(10,1)</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q17" s="8"/>
+    </row>
+    <row r="18" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -11469,15 +11816,17 @@
       <c r="E18" t="s">
         <v>156</v>
       </c>
+      <c r="H18" s="8"/>
       <c r="I18" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="J18" t="e" cm="1" vm="12">
+      <c r="J18" s="7" t="e" cm="1" vm="12">
         <f t="array" ref="J18">_xlfn._xlws.PY(11,1)</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q18" s="8"/>
+    </row>
+    <row r="19" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -11493,8 +11842,10 @@
       <c r="E19" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H19" s="8"/>
+      <c r="Q19" s="8"/>
+    </row>
+    <row r="20" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -11510,6 +11861,7 @@
       <c r="E20" t="s">
         <v>157</v>
       </c>
+      <c r="H20" s="8"/>
       <c r="I20" s="4" t="s">
         <v>162</v>
       </c>
@@ -11520,8 +11872,9 @@
       <c r="N20" s="4"/>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
-    </row>
-    <row r="21" spans="1:16" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="Q20" s="8"/>
+    </row>
+    <row r="21" spans="1:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -11537,8 +11890,10 @@
       <c r="E21" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H21" s="8"/>
+      <c r="Q21" s="8"/>
+    </row>
+    <row r="22" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -11554,15 +11909,17 @@
       <c r="E22" t="s">
         <v>158</v>
       </c>
+      <c r="H22" s="8"/>
       <c r="I22" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="J22" t="e" cm="1" vm="13">
+      <c r="J22" s="7" t="e" cm="1" vm="13">
         <f t="array" ref="J22">_xlfn._xlws.PY(12,1)</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q22" s="8"/>
+    </row>
+    <row r="23" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -11578,15 +11935,17 @@
       <c r="E23" t="s">
         <v>155</v>
       </c>
+      <c r="H23" s="8"/>
       <c r="I23" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="J23" t="e" cm="1" vm="14">
+      <c r="J23" s="7" t="e" cm="1" vm="14">
         <f t="array" ref="J23">_xlfn._xlws.PY(13,1)</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q23" s="8"/>
+    </row>
+    <row r="24" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -11602,15 +11961,17 @@
       <c r="E24" t="s">
         <v>157</v>
       </c>
+      <c r="H24" s="8"/>
       <c r="I24" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="J24" t="e" cm="1" vm="15">
+      <c r="J24" s="7" t="e" cm="1" vm="15">
         <f t="array" ref="J24">_xlfn._xlws.PY(14,1)</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q24" s="8"/>
+    </row>
+    <row r="25" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -11626,15 +11987,17 @@
       <c r="E25" t="s">
         <v>156</v>
       </c>
+      <c r="H25" s="8"/>
       <c r="I25" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="J25" t="e" cm="1" vm="16">
+      <c r="J25" s="7" t="e" cm="1" vm="16">
         <f t="array" ref="J25">_xlfn._xlws.PY(15,1)</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q25" s="8"/>
+    </row>
+    <row r="26" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -11650,15 +12013,17 @@
       <c r="E26" t="s">
         <v>155</v>
       </c>
+      <c r="H26" s="8"/>
       <c r="I26" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="J26" t="e" cm="1" vm="17">
+      <c r="J26" s="7" t="e" cm="1" vm="17">
         <f t="array" ref="J26">_xlfn._xlws.PY(16,1)</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q26" s="8"/>
+    </row>
+    <row r="27" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -11674,15 +12039,17 @@
       <c r="E27" t="s">
         <v>156</v>
       </c>
+      <c r="H27" s="8"/>
       <c r="I27" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="J27" t="e" cm="1" vm="18">
+      <c r="J27" s="7" t="e" cm="1" vm="18">
         <f t="array" ref="J27">_xlfn._xlws.PY(17,1)</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q27" s="8"/>
+    </row>
+    <row r="28" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -11698,8 +12065,10 @@
       <c r="E28" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H28" s="8"/>
+      <c r="Q28" s="8"/>
+    </row>
+    <row r="29" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -11715,6 +12084,7 @@
       <c r="E29" t="s">
         <v>156</v>
       </c>
+      <c r="H29" s="8"/>
       <c r="I29" s="4" t="s">
         <v>163</v>
       </c>
@@ -11725,8 +12095,9 @@
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
-    </row>
-    <row r="30" spans="1:16" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="Q29" s="8"/>
+    </row>
+    <row r="30" spans="1:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -11742,8 +12113,10 @@
       <c r="E30" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H30" s="8"/>
+      <c r="Q30" s="8"/>
+    </row>
+    <row r="31" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -11759,15 +12132,17 @@
       <c r="E31" t="s">
         <v>156</v>
       </c>
+      <c r="H31" s="8"/>
       <c r="I31" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="J31" t="e" cm="1" vm="19">
+      <c r="J31" s="7" t="e" cm="1" vm="19">
         <f t="array" ref="J31">_xlfn._xlws.PY(18,1)</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q31" s="8"/>
+    </row>
+    <row r="32" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -11783,8 +12158,10 @@
       <c r="E32" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H32" s="8"/>
+      <c r="Q32" s="8"/>
+    </row>
+    <row r="33" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -11800,6 +12177,7 @@
       <c r="E33" t="s">
         <v>155</v>
       </c>
+      <c r="H33" s="8"/>
       <c r="I33" s="4" t="s">
         <v>164</v>
       </c>
@@ -11810,8 +12188,9 @@
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
-    </row>
-    <row r="34" spans="1:16" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="Q33" s="8"/>
+    </row>
+    <row r="34" spans="1:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -11827,8 +12206,10 @@
       <c r="E34" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H34" s="8"/>
+      <c r="Q34" s="8"/>
+    </row>
+    <row r="35" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -11844,15 +12225,17 @@
       <c r="E35" t="s">
         <v>158</v>
       </c>
+      <c r="H35" s="8"/>
       <c r="I35" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="J35" t="e" cm="1" vm="20">
+      <c r="J35" s="7" t="e" cm="1" vm="20">
         <f t="array" ref="J35">_xlfn._xlws.PY(19,1)</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q35" s="8"/>
+    </row>
+    <row r="36" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -11868,8 +12251,10 @@
       <c r="E36" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H36" s="8"/>
+      <c r="Q36" s="8"/>
+    </row>
+    <row r="37" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -11885,13 +12270,20 @@
       <c r="E37" t="s">
         <v>158</v>
       </c>
+      <c r="H37" s="8"/>
       <c r="I37" s="4" t="s">
         <v>165</v>
       </c>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
-    </row>
-    <row r="38" spans="1:16" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="8"/>
+    </row>
+    <row r="38" spans="1:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -11907,8 +12299,10 @@
       <c r="E38" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H38" s="8"/>
+      <c r="Q38" s="8"/>
+    </row>
+    <row r="39" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -11924,15 +12318,17 @@
       <c r="E39" t="s">
         <v>156</v>
       </c>
+      <c r="H39" s="8"/>
       <c r="I39" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="J39" t="e" cm="1" vm="21">
+      <c r="J39" s="7" t="e" cm="1" vm="21">
         <f t="array" ref="J39">_xlfn._xlws.PY(20,1)</f>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q39" s="8"/>
+    </row>
+    <row r="40" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -11948,8 +12344,10 @@
       <c r="E40" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="41" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H40" s="8"/>
+      <c r="Q40" s="8"/>
+    </row>
+    <row r="41" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -11965,11 +12363,20 @@
       <c r="E41" t="s">
         <v>155</v>
       </c>
+      <c r="H41" s="8"/>
       <c r="I41" s="4" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="42" spans="1:16" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="O41" s="3"/>
+      <c r="P41" s="3"/>
+      <c r="Q41" s="8"/>
+    </row>
+    <row r="42" spans="1:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -11985,8 +12392,10 @@
       <c r="E42" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H42" s="8"/>
+      <c r="Q42" s="8"/>
+    </row>
+    <row r="43" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>46</v>
       </c>
@@ -12002,8 +12411,10 @@
       <c r="E43" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H43" s="8"/>
+      <c r="Q43" s="8"/>
+    </row>
+    <row r="44" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -12019,8 +12430,10 @@
       <c r="E44" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H44" s="8"/>
+      <c r="Q44" s="8"/>
+    </row>
+    <row r="45" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>48</v>
       </c>
@@ -12036,8 +12449,10 @@
       <c r="E45" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H45" s="8"/>
+      <c r="Q45" s="8"/>
+    </row>
+    <row r="46" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -12053,8 +12468,10 @@
       <c r="E46" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H46" s="8"/>
+      <c r="Q46" s="8"/>
+    </row>
+    <row r="47" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -12070,8 +12487,10 @@
       <c r="E47" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H47" s="8"/>
+      <c r="Q47" s="8"/>
+    </row>
+    <row r="48" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -12087,8 +12506,10 @@
       <c r="E48" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H48" s="8"/>
+      <c r="Q48" s="8"/>
+    </row>
+    <row r="49" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -12104,8 +12525,10 @@
       <c r="E49" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H49" s="8"/>
+      <c r="Q49" s="8"/>
+    </row>
+    <row r="50" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -12121,8 +12544,10 @@
       <c r="E50" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H50" s="8"/>
+      <c r="Q50" s="8"/>
+    </row>
+    <row r="51" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>54</v>
       </c>
@@ -12138,8 +12563,10 @@
       <c r="E51" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H51" s="8"/>
+      <c r="Q51" s="8"/>
+    </row>
+    <row r="52" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>55</v>
       </c>
@@ -12155,8 +12582,10 @@
       <c r="E52" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H52" s="8"/>
+      <c r="Q52" s="8"/>
+    </row>
+    <row r="53" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>56</v>
       </c>
@@ -12172,8 +12601,10 @@
       <c r="E53" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H53" s="8"/>
+      <c r="Q53" s="8"/>
+    </row>
+    <row r="54" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>57</v>
       </c>
@@ -12189,8 +12620,10 @@
       <c r="E54" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H54" s="8"/>
+      <c r="Q54" s="8"/>
+    </row>
+    <row r="55" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>58</v>
       </c>
@@ -12206,8 +12639,10 @@
       <c r="E55" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H55" s="8"/>
+      <c r="Q55" s="8"/>
+    </row>
+    <row r="56" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>59</v>
       </c>
@@ -12223,8 +12658,10 @@
       <c r="E56" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H56" s="8"/>
+      <c r="Q56" s="8"/>
+    </row>
+    <row r="57" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>60</v>
       </c>
@@ -12240,8 +12677,10 @@
       <c r="E57" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H57" s="8"/>
+      <c r="Q57" s="8"/>
+    </row>
+    <row r="58" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>61</v>
       </c>
@@ -12257,8 +12696,10 @@
       <c r="E58" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H58" s="8"/>
+      <c r="Q58" s="8"/>
+    </row>
+    <row r="59" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>62</v>
       </c>
@@ -12274,8 +12715,10 @@
       <c r="E59" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H59" s="8"/>
+      <c r="Q59" s="8"/>
+    </row>
+    <row r="60" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>63</v>
       </c>
@@ -12291,8 +12734,10 @@
       <c r="E60" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H60" s="8"/>
+      <c r="Q60" s="8"/>
+    </row>
+    <row r="61" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>64</v>
       </c>
@@ -12308,8 +12753,10 @@
       <c r="E61" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H61" s="8"/>
+      <c r="Q61" s="8"/>
+    </row>
+    <row r="62" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>65</v>
       </c>
@@ -12325,8 +12772,10 @@
       <c r="E62" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H62" s="8"/>
+      <c r="Q62" s="8"/>
+    </row>
+    <row r="63" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>66</v>
       </c>
@@ -12342,8 +12791,10 @@
       <c r="E63" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H63" s="8"/>
+      <c r="Q63" s="8"/>
+    </row>
+    <row r="64" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>67</v>
       </c>
@@ -12359,8 +12810,10 @@
       <c r="E64" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H64" s="8"/>
+      <c r="Q64" s="8"/>
+    </row>
+    <row r="65" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>68</v>
       </c>
@@ -12376,8 +12829,18 @@
       <c r="E65" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H65" s="8"/>
+      <c r="I65" s="8"/>
+      <c r="J65" s="8"/>
+      <c r="K65" s="8"/>
+      <c r="L65" s="8"/>
+      <c r="M65" s="8"/>
+      <c r="N65" s="8"/>
+      <c r="O65" s="8"/>
+      <c r="P65" s="8"/>
+      <c r="Q65" s="8"/>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>69</v>
       </c>
@@ -12394,7 +12857,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>70</v>
       </c>
@@ -12411,7 +12874,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>71</v>
       </c>
@@ -12428,7 +12891,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>72</v>
       </c>
@@ -12445,7 +12908,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>73</v>
       </c>
@@ -12462,7 +12925,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>74</v>
       </c>
@@ -12479,7 +12942,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>75</v>
       </c>
@@ -12496,7 +12959,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>76</v>
       </c>
@@ -12513,7 +12976,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>77</v>
       </c>
@@ -12530,7 +12993,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>78</v>
       </c>
@@ -12547,7 +13010,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>79</v>
       </c>
@@ -12564,7 +13027,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>80</v>
       </c>
@@ -12581,7 +13044,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>81</v>
       </c>
@@ -12598,7 +13061,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>82</v>
       </c>
@@ -12615,7 +13078,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>83</v>
       </c>
@@ -12990,7 +13453,10 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E101">
+    <sortCondition sortBy="cellColor" ref="A6:A101"/>
+  </sortState>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
chore: remove obsolete Excel files from the repository
</commit_message>
<xml_diff>
--- a/TASK_3/TAsk_3-Files.xlsx
+++ b/TASK_3/TAsk_3-Files.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/midhun/Developer/Git/Orion_Intern_Journey/TASK_3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FD73F8-A81A-0146-B081-B836AC7568EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE44178-7167-F347-AABD-896727C718AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="10062025" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="13062025" sheetId="4" r:id="rId4"/>
     <sheet name="14062025" sheetId="5" r:id="rId5"/>
     <sheet name="15062025" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="5">'15062025'!$H$1:$Q$64</definedName>
@@ -2001,7 +2002,7 @@
   <rv s="2">
     <v>&lt;class 'PIL.PngImagePlugin.PngImageFile'&gt;</v>
     <v>PngImageFile</v>
-    <v>&lt;PIL.PngImagePlugin.PngImageFile image mode=RGBA size=989x989 at 0x7F99DA0FB290&gt;</v>
+    <v>&lt;PIL.PngImagePlugin.PngImageFile image mode=RGBA size=989x989 at 0x7FDAA43A43B0&gt;</v>
     <v>56</v>
     <v>2</v>
   </rv>
@@ -9364,7 +9365,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{282EAF0B-A46B-0443-A423-FB0FE8A81679}">
   <dimension ref="A1:S101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
@@ -11316,8 +11317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1345756A-7B60-E14F-9547-EADEB936F73C}">
   <dimension ref="A1:Q101"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="T29" sqref="T29"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="35" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13461,4 +13462,18 @@
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3F56E65-4E3F-2945-92B5-78A11E7B0089}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
chore: update TASK_3-Files.xlsx with new data
</commit_message>
<xml_diff>
--- a/TASK_3/TAsk_3-Files.xlsx
+++ b/TASK_3/TAsk_3-Files.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/midhun/Developer/Git/Orion_Intern_Journey/TASK_3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE44178-7167-F347-AABD-896727C718AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44961CC9-59F6-0344-8E61-3D4C1C99C87C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2002,7 +2002,7 @@
   <rv s="2">
     <v>&lt;class 'PIL.PngImagePlugin.PngImageFile'&gt;</v>
     <v>PngImageFile</v>
-    <v>&lt;PIL.PngImagePlugin.PngImageFile image mode=RGBA size=989x989 at 0x7FDAA43A43B0&gt;</v>
+    <v>&lt;PIL.PngImagePlugin.PngImageFile image mode=RGBA size=989x989 at 0x7F519CAEE000&gt;</v>
     <v>56</v>
     <v>2</v>
   </rv>
@@ -11317,8 +11317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1345756A-7B60-E14F-9547-EADEB936F73C}">
   <dimension ref="A1:Q101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="35" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="86" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>